<commit_message>
Added solar and occupancy meter list functionality
The solar and occupancy meter lists can be populated on startup. Can also interact with the UI in ConvVR to load these meter lists.
</commit_message>
<xml_diff>
--- a/Unity-Environments/Conv_CaseStudy/Assets/Resources/MeterNames_20220328.xlsx
+++ b/Unity-Environments/Conv_CaseStudy/Assets/Resources/MeterNames_20220328.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anro1\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Desktop\Masters-Case-Study\Unity-Environments\Conv_CaseStudy\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84F755E2-6534-438E-8CC9-5FBAE6DD1AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F078D5B-0493-4A58-9C59-0741151070B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{BD2201DA-CF77-4F5D-B6D4-E19D905DD302}"/>
+    <workbookView xWindow="-28920" yWindow="-5970" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{BD2201DA-CF77-4F5D-B6D4-E19D905DD302}"/>
   </bookViews>
   <sheets>
     <sheet name="Energy" sheetId="1" r:id="rId1"/>
@@ -691,29 +691,29 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -778,7 +778,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -843,7 +843,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -908,7 +908,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -973,7 +973,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1753,7 +1753,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1961,27 +1961,27 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -2120,31 +2120,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A93FEF5-8629-41AD-8AC9-A3A5A6424C9D}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>92</v>
       </c>

</xml_diff>